<commit_message>
Organizando el continuos notebook
</commit_message>
<xml_diff>
--- a/Binary/Matriz selección de variablesv2.xlsx
+++ b/Binary/Matriz selección de variablesv2.xlsx
@@ -8,17 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\OneDrive - CELSIA S.A E.S.P\Maestría\Metodos estadisticos avanzados\Competencia\Binary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{41363F96-E0F7-ED4D-8E09-02F365787421}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{094458DE-CC35-437B-B1BB-F922A1BA5629}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="8_{41363F96-E0F7-ED4D-8E09-02F365787421}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{F50A924B-158F-4F6B-B27C-3ED801345212}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja2" sheetId="2" state="hidden" r:id="rId1"/>
     <sheet name="sin estand" sheetId="3" r:id="rId2"/>
     <sheet name="estandariz" sheetId="4" r:id="rId3"/>
-    <sheet name="tablas" sheetId="6" r:id="rId4"/>
-    <sheet name="spike and slab" sheetId="5" r:id="rId5"/>
-    <sheet name="corridas" sheetId="7" r:id="rId6"/>
+    <sheet name="Hoja3" sheetId="9" r:id="rId4"/>
+    <sheet name="Hoja1" sheetId="8" r:id="rId5"/>
+    <sheet name="tablas" sheetId="6" r:id="rId6"/>
+    <sheet name="spike and slab" sheetId="5" r:id="rId7"/>
+    <sheet name="corridas" sheetId="7" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">estandariz!$A$1:$R$37</definedName>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="124">
   <si>
     <t>PROMEDIO</t>
   </si>
@@ -403,6 +405,12 @@
   </si>
   <si>
     <t>DESVEST</t>
+  </si>
+  <si>
+    <t>Variables</t>
+  </si>
+  <si>
+    <t>Probabilidad</t>
   </si>
 </sst>
 </file>
@@ -8865,16 +8873,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9A59654-933E-264A-BE3D-BC19FDB1E4BB}">
   <dimension ref="A1:T57"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q6" sqref="Q6"/>
+    <sheetView showGridLines="0" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="R2" activeCellId="1" sqref="A2:A35 R2:R35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="7.42578125" style="30" customWidth="1"/>
-    <col min="2" max="3" width="9.28515625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" style="7" customWidth="1"/>
-    <col min="5" max="17" width="9.28515625" style="3" customWidth="1"/>
+    <col min="2" max="3" width="9.28515625" style="3" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" style="7" hidden="1" customWidth="1"/>
+    <col min="5" max="17" width="9.28515625" style="3" hidden="1" customWidth="1"/>
     <col min="18" max="18" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -10399,6 +10407,327 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB9189B3-EDC6-40F0-83F0-990F7EE4251D}">
+  <dimension ref="A1:B35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="16">
+        <v>1</v>
+      </c>
+      <c r="B2" s="15">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="29">
+        <v>2</v>
+      </c>
+      <c r="B3" s="15">
+        <v>0.73333333333333328</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="29">
+        <v>3</v>
+      </c>
+      <c r="B4" s="15">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="28">
+        <v>4</v>
+      </c>
+      <c r="B5" s="15">
+        <v>0.73333333333333328</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="29">
+        <v>5</v>
+      </c>
+      <c r="B6" s="15">
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="28">
+        <v>6</v>
+      </c>
+      <c r="B7" s="15">
+        <v>0.46666666666666667</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="28">
+        <v>7</v>
+      </c>
+      <c r="B8" s="15">
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="28">
+        <v>8</v>
+      </c>
+      <c r="B9" s="15">
+        <v>0.46666666666666667</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="29">
+        <v>9</v>
+      </c>
+      <c r="B10" s="15">
+        <v>0.46666666666666667</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="16">
+        <v>10</v>
+      </c>
+      <c r="B11" s="15">
+        <v>0.8666666666666667</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="29">
+        <v>11</v>
+      </c>
+      <c r="B12" s="15">
+        <v>0.73333333333333328</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="16">
+        <v>12</v>
+      </c>
+      <c r="B13" s="15">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="29">
+        <v>13</v>
+      </c>
+      <c r="B14" s="15">
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="28">
+        <v>14</v>
+      </c>
+      <c r="B15" s="15">
+        <v>0.53333333333333333</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="29">
+        <v>15</v>
+      </c>
+      <c r="B16" s="15">
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="29">
+        <v>16</v>
+      </c>
+      <c r="B17" s="15">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="16">
+        <v>17</v>
+      </c>
+      <c r="B18" s="15">
+        <v>0.93333333333333335</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="29">
+        <v>18</v>
+      </c>
+      <c r="B19" s="15">
+        <v>0.53333333333333333</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="29">
+        <v>19</v>
+      </c>
+      <c r="B20" s="15">
+        <v>0.46666666666666667</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="29">
+        <v>20</v>
+      </c>
+      <c r="B21" s="15">
+        <v>0.26666666666666666</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="29">
+        <v>21</v>
+      </c>
+      <c r="B22" s="15">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="29">
+        <v>22</v>
+      </c>
+      <c r="B23" s="15">
+        <v>0.53333333333333333</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="16">
+        <v>23</v>
+      </c>
+      <c r="B24" s="15">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="29">
+        <v>24</v>
+      </c>
+      <c r="B25" s="15">
+        <v>0.53333333333333333</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="29">
+        <v>25</v>
+      </c>
+      <c r="B26" s="15">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="28">
+        <v>26</v>
+      </c>
+      <c r="B27" s="15">
+        <v>0.26666666666666666</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="28">
+        <v>27</v>
+      </c>
+      <c r="B28" s="15">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="28">
+        <v>28</v>
+      </c>
+      <c r="B29" s="15">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="29">
+        <v>29</v>
+      </c>
+      <c r="B30" s="15">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" s="28">
+        <v>30</v>
+      </c>
+      <c r="B31" s="15">
+        <v>0.53333333333333333</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" s="28">
+        <v>31</v>
+      </c>
+      <c r="B32" s="15">
+        <v>0.26666666666666666</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="29">
+        <v>32</v>
+      </c>
+      <c r="B33" s="15">
+        <v>0.53333333333333333</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" s="28">
+        <v>33</v>
+      </c>
+      <c r="B34" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" s="28">
+        <v>34</v>
+      </c>
+      <c r="B35" s="15">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B2:B35">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CC2CEDA-DEFC-4370-B810-37BD78F2D754}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D2E5B58-D664-294D-9F7F-E7605796B887}">
   <dimension ref="C4:N44"/>
   <sheetViews>
@@ -10790,7 +11119,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{069B4A5F-AFA7-B444-9935-2736A981AFCA}">
   <dimension ref="B2:F36"/>
   <sheetViews>
@@ -11454,7 +11783,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A47A7FB8-1D29-F646-8A4F-B92669D8C45C}">
   <dimension ref="A3:V81"/>
   <sheetViews>

</xml_diff>